<commit_message>
test(result): add result file
</commit_message>
<xml_diff>
--- a/wgcpy/result/feats_seletor_result.xlsx
+++ b/wgcpy/result/feats_seletor_result.xlsx
@@ -669,7 +669,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -729,7 +729,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -749,7 +749,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -769,7 +769,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -789,7 +789,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
@@ -829,7 +829,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -849,7 +849,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -869,7 +869,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
@@ -939,7 +939,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -979,7 +979,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -999,7 +999,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -1019,7 +1019,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -1039,7 +1039,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -1059,7 +1059,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>

</xml_diff>